<commit_message>
Continue working with diff report
</commit_message>
<xml_diff>
--- a/templates/diff.xlsx
+++ b/templates/diff.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Electron\git-log-viewer\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Electron\git-log-viewer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
-    <sheet name="Commits" sheetId="1" r:id="rId1"/>
+    <sheet name="Diff" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Commits!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Diff!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,23 +33,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Committer name</t>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>File path</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Committer email</t>
+    <t>Diff file</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Commit message</t>
+    <t>Need to create test case?</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Hash</t>
+    <t>Has diffirences?</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -60,14 +60,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -434,33 +434,33 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="7.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="72.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="39" style="2" customWidth="1"/>
+    <col min="3" max="3" width="89.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1">
+    <row r="1" spans="1:6" ht="32.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>